<commit_message>
updating data labeling script, and adding exit column deletions
</commit_message>
<xml_diff>
--- a/data_names.xlsx
+++ b/data_names.xlsx
@@ -604,96 +604,96 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PROTEO_EOTAXIN_HUMAN</t>
+          <t>PROTEOMICS_EOTAXIN (HUMAN)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Incompatible</t>
+          <t>Eotaxin, human</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PROTEO_IFN_Y_HUMAN</t>
+          <t>PROTEOMICS_IFN-Y (HUMAN)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Incompatible</t>
+          <t>Interferon y, human</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PROTEO_IL_15</t>
+          <t>PROTEOMICS_IL-15</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Incompatible</t>
+          <t>Interleukin-15</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PROTEO_MCP_4_HUMAN</t>
+          <t>PROTEOMICS_MCP-4 (HUMAN)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Incompatible</t>
+          <t>Monocyte chemotactic protein-4, human</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PROTEO_MDC_HUMAN</t>
+          <t>PROTEOMICS_MDC (HUMAN)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Incompatible</t>
+          <t>Myeloid dentritic cells, human</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PROTEO_MIP_1A_HUMAN</t>
+          <t>PROTEOMICS_MIP-1A (HUMAN)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Incompatible</t>
+          <t>Macrophage Inflammatory Protein 1a, human</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PROTEO_SAA</t>
+          <t>PROTEOMICS_SAA</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Incompatible</t>
+          <t>Serum amyloid A</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PROTEO_VEGF_ANGIO_PLATE</t>
+          <t>PROTEOMICS_VEGF- ANGIO PLATE</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Incompatible</t>
+          <t>Vascular endothelial growth factor angio plate</t>
         </is>
       </c>
     </row>

</xml_diff>